<commit_message>
Lam khung them thong tin san pham
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Web\shopping-cart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\Học\Học kì 4\Web\Shopping-cart-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA802E06-7224-424F-BF19-04790DECDF67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48806FC-3150-47BC-BDAC-1780C6634D5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2FF8D325-9289-4B3A-B7DB-16E5F351C26F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FF8D325-9289-4B3A-B7DB-16E5F351C26F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -556,29 +556,29 @@
   <dimension ref="B1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="33.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="4" customWidth="1"/>
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -589,7 +589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -600,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -609,7 +609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -618,7 +618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
@@ -627,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
@@ -636,7 +636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
@@ -645,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
@@ -654,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
@@ -663,7 +663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -672,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
@@ -681,17 +681,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
@@ -699,109 +699,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xoa mot so phan cong
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\Học\Học kì 4\Web\Shopping-cart-web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAY\Downloads\Shopping-cart-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48806FC-3150-47BC-BDAC-1780C6634D5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FF8D325-9289-4B3A-B7DB-16E5F351C26F}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Trang chính</t>
   </si>
@@ -133,9 +132,6 @@
   </si>
   <si>
     <t>Danh sách sản phẩm</t>
-  </si>
-  <si>
-    <t>Quản lí category sản phẩm</t>
   </si>
   <si>
     <t>Chi tiết sản phẩm</t>
@@ -150,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,7 +237,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -552,33 +548,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB43815-C2F2-4FA6-8CDE-7BD59305C443}">
-  <dimension ref="B1:D39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="33.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -589,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -600,7 +596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -609,7 +605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -618,191 +614,182 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update phân công công việc
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAY\Downloads\Shopping-cart-web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Web\shopping-cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC2E1C6-15E7-4E28-B78A-DFF91E4FCA13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Trang chính</t>
   </si>
@@ -146,12 +138,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -237,7 +229,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -548,33 +540,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.75" style="4" customWidth="1"/>
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -585,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -596,7 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -605,7 +597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -614,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -623,7 +615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -632,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
@@ -641,7 +633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -650,7 +642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
@@ -659,7 +651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -668,17 +660,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -686,109 +678,111 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="6"/>
     </row>
   </sheetData>

</xml_diff>